<commit_message>
IO file mapping adjustments to match with BIFUbC (there are some ISIC codes that were combined with others in BIFUbC, made that consistent for relevant IO files)
</commit_message>
<xml_diff>
--- a/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
+++ b/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\io-model\BECbIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\EPS Models\EU EPS\InputData\io-model\BECbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191AFAF-EF1E-4F19-A44D-C62CF07F070C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B74C56-03DC-439B-8657-37A98977B5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="2055" windowWidth="19305" windowHeight="14430" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="465" windowWidth="26460" windowHeight="7800" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22965,8 +22965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CDC51E-E505-4236-84C2-F185FBAFFCE4}">
   <dimension ref="A1:Z123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27995,8 +27995,8 @@
   </sheetPr>
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28155,8 +28155,7 @@
         <v>11185172707.53479</v>
       </c>
       <c r="E2">
-        <f>'OECD VAL EU'!E35*10^6*About!$A$36</f>
-        <v>7828450490.4205198</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <f>'OECD VAL EU'!F35*10^6*About!$A$36</f>
@@ -28191,8 +28190,7 @@
         <v>59544488888.638145</v>
       </c>
       <c r="N2">
-        <f>'OECD VAL EU'!M35*10^6*About!$A$36</f>
-        <v>56454646705.991539</v>
+        <v>0</v>
       </c>
       <c r="O2" s="52">
         <f>'OECD VAL US'!N9*10^6*About!$A$36*('EU Data for ISIC Splits'!J10/SUM('EU Data for ISIC Splits'!J10:K10))</f>
@@ -28211,32 +28209,28 @@
         <v>11165793403.897251</v>
       </c>
       <c r="S2">
-        <f>'OECD VAL EU'!P35*10^6*About!$A$36</f>
-        <v>115189611484.28172</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <f>'OECD VAL EU'!Q35*10^6*About!$A$36</f>
-        <v>54677388222.06002</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <f>'OECD VAL EU'!R35*10^6*About!$A$36</f>
-        <v>61353004962.310722</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <f>'OECD VAL EU'!S35*10^6*About!$A$36</f>
-        <v>143027380027.69415</v>
+        <f>'OECD VAL EU'!S35*10^6*About!$A$36+'OECD VAL EU'!R35*10^6*About!$A$36+'OECD VAL EU'!Q35*10^6*About!$A$36+'OECD VAL EU'!P35*10^6*About!$A$36</f>
+        <v>374247384696.34662</v>
       </c>
       <c r="W2">
-        <f>'OECD VAL EU'!T35*10^6*About!$A$36</f>
-        <v>121755853419.62813</v>
+        <f>'OECD VAL EU'!T35*10^6*About!$A$36+'OECD VAL EU'!U35*10^6*About!$A$36</f>
+        <v>154811957053.37592</v>
       </c>
       <c r="X2">
-        <f>'OECD VAL EU'!U35*10^6*About!$A$36</f>
-        <v>33056103633.747795</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <f>'OECD VAL EU'!V35*10^6*About!$A$36</f>
-        <v>115208284758.93289</v>
+        <f>'OECD VAL EU'!V35*10^6*About!$A$36+'OECD VAL EU'!M35*10^6*About!$A$36+'OECD VAL EU'!X35*10^6*About!$A$36+'OECD VAL EU'!E35*10^6*About!$A$36</f>
+        <v>512209373798.3266</v>
       </c>
       <c r="Z2" s="52">
         <f>'OECD VAL US'!W9*10^6*About!$A$36*('EU Data for ISIC Splits'!P10/SUM('EU Data for ISIC Splits'!P10:R10))</f>
@@ -28251,8 +28245,7 @@
         <v>54600680708.644234</v>
       </c>
       <c r="AC2">
-        <f>'OECD VAL EU'!X35*10^6*About!$A$36</f>
-        <v>332717991842.98163</v>
+        <v>0</v>
       </c>
       <c r="AD2">
         <f>'OECD VAL EU'!Y35*10^6*About!$A$36</f>
@@ -28318,12 +28311,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28550,20 +28545,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E46C6E-E7F4-4336-B2D9-D075C882516C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51831F5-BBC8-4C0F-87D0-DEE41C3CA568}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28588,12 +28584,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51831F5-BBC8-4C0F-87D0-DEE41C3CA568}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E46C6E-E7F4-4336-B2D9-D075C882516C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "IO file mapping adjustments to match with BIFUbC (there are some ISIC codes that were combined with others in BIFUbC, made that consistent for relevant IO files)"
This reverts commit d33e4eb010bec651cd626f036e5182f36d18073b.
</commit_message>
<xml_diff>
--- a/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
+++ b/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\EPS Models\EU EPS\InputData\io-model\BECbIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\io-model\BECbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B74C56-03DC-439B-8657-37A98977B5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191AFAF-EF1E-4F19-A44D-C62CF07F070C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="465" windowWidth="26460" windowHeight="7800" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="2055" windowWidth="19305" windowHeight="14430" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22965,8 +22965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CDC51E-E505-4236-84C2-F185FBAFFCE4}">
   <dimension ref="A1:Z123"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27995,8 +27995,8 @@
   </sheetPr>
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28155,7 +28155,8 @@
         <v>11185172707.53479</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>'OECD VAL EU'!E35*10^6*About!$A$36</f>
+        <v>7828450490.4205198</v>
       </c>
       <c r="F2">
         <f>'OECD VAL EU'!F35*10^6*About!$A$36</f>
@@ -28190,7 +28191,8 @@
         <v>59544488888.638145</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <f>'OECD VAL EU'!M35*10^6*About!$A$36</f>
+        <v>56454646705.991539</v>
       </c>
       <c r="O2" s="52">
         <f>'OECD VAL US'!N9*10^6*About!$A$36*('EU Data for ISIC Splits'!J10/SUM('EU Data for ISIC Splits'!J10:K10))</f>
@@ -28209,28 +28211,32 @@
         <v>11165793403.897251</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <f>'OECD VAL EU'!P35*10^6*About!$A$36</f>
+        <v>115189611484.28172</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <f>'OECD VAL EU'!Q35*10^6*About!$A$36</f>
+        <v>54677388222.06002</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <f>'OECD VAL EU'!R35*10^6*About!$A$36</f>
+        <v>61353004962.310722</v>
       </c>
       <c r="V2">
-        <f>'OECD VAL EU'!S35*10^6*About!$A$36+'OECD VAL EU'!R35*10^6*About!$A$36+'OECD VAL EU'!Q35*10^6*About!$A$36+'OECD VAL EU'!P35*10^6*About!$A$36</f>
-        <v>374247384696.34662</v>
+        <f>'OECD VAL EU'!S35*10^6*About!$A$36</f>
+        <v>143027380027.69415</v>
       </c>
       <c r="W2">
-        <f>'OECD VAL EU'!T35*10^6*About!$A$36+'OECD VAL EU'!U35*10^6*About!$A$36</f>
-        <v>154811957053.37592</v>
+        <f>'OECD VAL EU'!T35*10^6*About!$A$36</f>
+        <v>121755853419.62813</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <f>'OECD VAL EU'!U35*10^6*About!$A$36</f>
+        <v>33056103633.747795</v>
       </c>
       <c r="Y2">
-        <f>'OECD VAL EU'!V35*10^6*About!$A$36+'OECD VAL EU'!M35*10^6*About!$A$36+'OECD VAL EU'!X35*10^6*About!$A$36+'OECD VAL EU'!E35*10^6*About!$A$36</f>
-        <v>512209373798.3266</v>
+        <f>'OECD VAL EU'!V35*10^6*About!$A$36</f>
+        <v>115208284758.93289</v>
       </c>
       <c r="Z2" s="52">
         <f>'OECD VAL US'!W9*10^6*About!$A$36*('EU Data for ISIC Splits'!P10/SUM('EU Data for ISIC Splits'!P10:R10))</f>
@@ -28245,7 +28251,8 @@
         <v>54600680708.644234</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <f>'OECD VAL EU'!X35*10^6*About!$A$36</f>
+        <v>332717991842.98163</v>
       </c>
       <c r="AD2">
         <f>'OECD VAL EU'!Y35*10^6*About!$A$36</f>
@@ -28311,14 +28318,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28545,21 +28550,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51831F5-BBC8-4C0F-87D0-DEE41C3CA568}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E46C6E-E7F4-4336-B2D9-D075C882516C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28584,9 +28588,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E46C6E-E7F4-4336-B2D9-D075C882516C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51831F5-BBC8-4C0F-87D0-DEE41C3CA568}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>